<commit_message>
Update template and readme so app is usable for other timeframes
</commit_message>
<xml_diff>
--- a/quarterlyReports/MM-DD-YY report_template.xlsx
+++ b/quarterlyReports/MM-DD-YY report_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayalapp/Documents/coding_projects/dad_data_project/quarterlyReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383F02BE-BB20-3045-B9B3-CCE1A1D77F2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC382112-D767-154E-996D-2737A025BC87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13960" activeTab="1" xr2:uid="{87EF98BD-D16B-484A-BF1E-96723C7FF38B}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13960" xr2:uid="{87EF98BD-D16B-484A-BF1E-96723C7FF38B}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">Location: </t>
   </si>
   <si>
-    <t>DATE OF QUARTERLY REPORT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Item </t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">Site 9 </t>
+  </si>
+  <si>
+    <t>DATE OF REPORT</t>
   </si>
 </sst>
 </file>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10BA574-3245-D145-83BF-04093C567771}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,7 +516,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -524,135 +524,135 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N6" s="1"/>
     </row>
     <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D358D96D-32E9-6B4E-9143-C4025DE546D1}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -677,7 +677,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -685,69 +685,69 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>1211</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>789</v>
@@ -811,15 +811,15 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(5:5)</f>
@@ -828,7 +828,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <f>SUM(6:6)</f>

</xml_diff>